<commit_message>
merged ics and xlsx
</commit_message>
<xml_diff>
--- a/climbing_training_plan_clean.xlsx
+++ b/climbing_training_plan_clean.xlsx
@@ -124,16 +124,16 @@
     <t>Load</t>
   </si>
   <si>
-    <t>10.0 hours</t>
-  </si>
-  <si>
-    <t>8.0 hours</t>
-  </si>
-  <si>
-    <t>11.2 hours</t>
-  </si>
-  <si>
-    <t>10.5 hours</t>
+    <t>11.0 hours</t>
+  </si>
+  <si>
+    <t>9.0 hours</t>
+  </si>
+  <si>
+    <t>12.2 hours</t>
+  </si>
+  <si>
+    <t>11.5 hours</t>
   </si>
   <si>
     <t>0.0 hours</t>
@@ -172,17 +172,17 @@
     <t>Bouldering</t>
   </si>
   <si>
+    <t>4X4</t>
+  </si>
+  <si>
     <t>Max Bouldering</t>
-  </si>
-  <si>
-    <t>4X4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -212,6 +212,12 @@
     </font>
     <font>
       <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -295,7 +301,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -307,14 +313,18 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -835,23 +845,23 @@
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
     </row>
     <row r="7" spans="1:15">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="9" t="s">
         <v>42</v>
       </c>
       <c r="B7" s="8" t="s">
@@ -892,7 +902,7 @@
       </c>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="9" t="s">
         <v>43</v>
       </c>
       <c r="B8" s="8" t="s">
@@ -933,26 +943,26 @@
       </c>
     </row>
     <row r="9" spans="1:15">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
     </row>
     <row r="10" spans="1:15">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="12" t="s">
         <v>45</v>
       </c>
       <c r="B10" s="11" t="s">
@@ -993,7 +1003,7 @@
       </c>
     </row>
     <row r="11" spans="1:15">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="13" t="s">
         <v>46</v>
       </c>
       <c r="B11" s="11" t="s">
@@ -1010,155 +1020,155 @@
       </c>
     </row>
     <row r="12" spans="1:15">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="12"/>
-      <c r="O12" s="12"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
     </row>
     <row r="13" spans="1:15">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="H13" s="13" t="s">
+      <c r="H13" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="I13" s="13" t="s">
+      <c r="I13" s="15" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:15">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="H14" s="13" t="s">
+      <c r="H14" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="I14" s="13" t="s">
+      <c r="I14" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="K14" s="13" t="s">
+      <c r="K14" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="L14" s="13" t="s">
+      <c r="L14" s="15" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:15">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="E15" s="15" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:15">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="15"/>
-      <c r="O16" s="15"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
+      <c r="M16" s="19"/>
+      <c r="N16" s="19"/>
+      <c r="O16" s="19"/>
     </row>
     <row r="17" spans="1:13">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="F17" s="16" t="s">
+      <c r="C17" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="G17" s="16" t="s">
+      <c r="E17" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="H17" s="16" t="s">
+      <c r="I17" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="I17" s="16" t="s">
+      <c r="L17" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="J17" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="K17" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="L17" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="M17" s="16" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="18" spans="1:13">
-      <c r="A18" s="16" t="s">
+      <c r="A18" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="F18" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="E18" s="16" t="s">
+      <c r="G18" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="I18" s="16" t="s">
+      <c r="H18" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="L18" s="16" t="s">
+      <c r="I18" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="J18" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="K18" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="L18" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="M18" s="19" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>